<commit_message>
set font family, split DonMuaHang, format SoHoaDon, format template
</commit_message>
<xml_diff>
--- a/adg-server/src/main/resources/bidv/BẢNG KÊ SỬ DỤNG TIỀN VAY.xlsx
+++ b/adg-server/src/main/resources/bidv/BẢNG KÊ SỬ DỤNG TIỀN VAY.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luan.phm/engineering/Projects/ADongGroup/adg-services/adg-api/src/main/resources/bidv/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luan.phm/engineering/Projects/ADongGroup/adg-services/adg-server/src/main/resources/bidv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49DAE4C4-4B41-514D-A545-C7195B1B57C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F939AAF-8528-E44F-902E-251CA20EE765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32440" yWindow="4060" windowWidth="32440" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -300,9 +300,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -323,6 +320,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,7 +544,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -565,24 +565,24 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" ht="15">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
     </row>
     <row r="3" spans="1:6" ht="15">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
     </row>
     <row r="4" spans="1:6" ht="16">
       <c r="A4" s="2"/>
@@ -593,14 +593,14 @@
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" ht="19">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
     </row>
     <row r="6" spans="1:6" ht="16">
       <c r="A6" s="2"/>
@@ -611,14 +611,14 @@
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" ht="14">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
     </row>
     <row r="8" spans="1:6" ht="16">
       <c r="A8" s="3"/>
@@ -652,16 +652,16 @@
       <c r="A10" s="14"/>
       <c r="B10" s="15"/>
       <c r="C10" s="14"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
     </row>
     <row r="11" spans="1:6" ht="15">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
       <c r="D11" s="12"/>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
@@ -675,14 +675,14 @@
       <c r="F12" s="8"/>
     </row>
     <row r="13" spans="1:6" ht="14">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
     </row>
     <row r="14" spans="1:6" ht="15">
       <c r="A14" s="5"/>

</xml_diff>